<commit_message>
Some more data collection
</commit_message>
<xml_diff>
--- a/terrain/Report/Data/Formatted/AIConfigFormatted.xlsx
+++ b/terrain/Report/Data/Formatted/AIConfigFormatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lizardbot\terrain\Report\Data\Formatted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363970E8-4C59-4394-9069-C206A1FA2F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D81825D-B581-4048-A812-F261A09876D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7BCDFC9F-3AC9-4EF9-9723-35C36DFC9674}"/>
   </bookViews>
@@ -31,28 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,11 +469,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3C4000-5345-42F8-AAA4-25B00B30B4A9}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +489,7 @@
     <col min="11" max="11" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -545,12 +523,8 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="str" cm="1">
-        <f t="array" ref="M1:M22">_xlfn.UNIQUE(G:G)</f>
-        <v xml:space="preserve"> RecombinationRate</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -584,11 +558,8 @@
       <c r="K2">
         <v>9</v>
       </c>
-      <c r="M2">
-        <v>0.76650700000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -622,11 +593,8 @@
       <c r="K3" s="5">
         <v>9</v>
       </c>
-      <c r="M3">
-        <v>0.13700080000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -660,11 +628,8 @@
       <c r="K4">
         <v>13</v>
       </c>
-      <c r="M4">
-        <v>0.75480639999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -698,11 +663,8 @@
       <c r="K5">
         <v>11</v>
       </c>
-      <c r="M5">
-        <v>0.43900830000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -736,11 +698,8 @@
       <c r="K6" s="5">
         <v>9</v>
       </c>
-      <c r="M6">
-        <v>0.1545686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -774,11 +733,8 @@
       <c r="K7">
         <v>7</v>
       </c>
-      <c r="M7">
-        <v>0.12653539999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -812,11 +768,8 @@
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>0.18884970000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -850,11 +803,8 @@
       <c r="K9" s="5">
         <v>9</v>
       </c>
-      <c r="M9">
-        <v>0.10048609999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -888,11 +838,8 @@
       <c r="K10" s="5">
         <v>9</v>
       </c>
-      <c r="M10">
-        <v>0.88540960000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -926,11 +873,8 @@
       <c r="K11">
         <v>15</v>
       </c>
-      <c r="M11">
-        <v>9.1093430000000003E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -964,11 +908,8 @@
       <c r="K12" s="6">
         <v>9</v>
       </c>
-      <c r="M12">
-        <v>0.3957254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1002,11 +943,8 @@
       <c r="K13">
         <v>16</v>
       </c>
-      <c r="M13">
-        <v>0.42400149999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1040,11 +978,8 @@
       <c r="K14">
         <v>9</v>
       </c>
-      <c r="M14">
-        <v>0.29317880000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1078,11 +1013,8 @@
       <c r="K15">
         <v>9</v>
       </c>
-      <c r="M15">
-        <v>0.13745859999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1116,11 +1048,8 @@
       <c r="K16">
         <v>10</v>
       </c>
-      <c r="M16">
-        <v>0.50183420000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1154,11 +1083,8 @@
       <c r="K17">
         <v>19</v>
       </c>
-      <c r="M17">
-        <v>0.20910860000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1192,11 +1118,8 @@
       <c r="K18" s="5">
         <v>9</v>
       </c>
-      <c r="M18">
-        <v>1.6166449999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1230,11 +1153,8 @@
       <c r="K19">
         <v>19</v>
       </c>
-      <c r="M19">
-        <v>0.1216116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1268,11 +1188,8 @@
       <c r="K20">
         <v>2</v>
       </c>
-      <c r="M20">
-        <v>0.23403160000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1306,11 +1223,8 @@
       <c r="K21">
         <v>9</v>
       </c>
-      <c r="M21">
-        <v>0.8257333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1344,11 +1258,8 @@
       <c r="K22" s="5">
         <v>9</v>
       </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1383,7 +1294,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1418,7 +1329,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1453,7 +1364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1488,7 +1399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1523,7 +1434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1558,7 +1469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1593,7 +1504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1628,7 +1539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1663,7 +1574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1698,7 +1609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1766,36 +1677,6 @@
       </c>
       <c r="K34" s="6">
         <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>